<commit_message>
Update help command Bug fix on new connexion state management
</commit_message>
<xml_diff>
--- a/Translations.xlsx
+++ b/Translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="20055" windowHeight="12015" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="20055" windowHeight="12015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="En" sheetId="1" r:id="rId1"/>
@@ -883,9 +883,6 @@
     <t>- %s: execute shell instuction with root access if possible.</t>
   </si>
   <si>
-    <t>and you can paste links and open it with the appropriate application.</t>
-  </si>
-  <si>
     <t>chat_start_locating</t>
   </si>
   <si>
@@ -1102,9 +1099,6 @@
     <t>- %s: exécuter une commande shell avec les droits super administrateur si possible.</t>
   </si>
   <si>
-    <t>et coller les liens http pour les ouvrir dans le navigateur du téléphone.</t>
-  </si>
-  <si>
     <t>Error can\'t dial.</t>
   </si>
   <si>
@@ -1291,12 +1285,6 @@
     <t>Bienvenue dans GTalkSMS %s. Envoyer \"?\" pour afficher l\'aide.</t>
   </si>
   <si>
-    <t>- %s: envoie continue de liens Gmap pour localiser le téléphone jusqu\'à l\'envoie de la commande \"stop\".</t>
-  </si>
-  <si>
-    <t>- %s: faire sonner le téléphone jusqu\'à l\'envoie de la commande \"stop\".</t>
-  </si>
-  <si>
     <t>%1$d contacts trouvés pour \"%2$s\"</t>
   </si>
   <si>
@@ -1309,12 +1297,6 @@
     <t>Welcome to GTalkSMS %s. Send \"?\" for getting help.</t>
   </si>
   <si>
-    <t>- %s: sends you google map updates about the location of the phone until you send \"stop\".</t>
-  </si>
-  <si>
-    <t>- %s: rings the phone until you send \"stop\".</t>
-  </si>
-  <si>
     <t>%1$d contacts found for \"%2$s\"</t>
   </si>
   <si>
@@ -1346,6 +1328,24 @@
   </si>
   <si>
     <t>&amp;#xA0;de&amp;#xA0;</t>
+  </si>
+  <si>
+    <t>- %1$s: rings the phone until you send %2$s.</t>
+  </si>
+  <si>
+    <t>- %1$s: sends you google map updates about the location of the phone until you send %2$s.</t>
+  </si>
+  <si>
+    <t>- %1$s: envoie continue de liens Gmap pour localiser le téléphone jusqu\'à l\'envoie de la commande %2$s.</t>
+  </si>
+  <si>
+    <t>- %1$s: faire sonner le téléphone jusqu\'à l\'envoie de la commande %2$s.</t>
+  </si>
+  <si>
+    <t>et coller les liens %s pour les ouvrir dans le navigateur du téléphone.</t>
+  </si>
+  <si>
+    <t>and you can paste %s links and open it with the appropriate application.</t>
   </si>
 </sst>
 </file>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2384,7 +2384,7 @@
         <v>247</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2400,7 +2400,7 @@
         <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2413,7 +2413,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B91" t="s">
         <v>255</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B92" t="s">
         <v>256</v>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B93" t="s">
         <v>257</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B94" t="s">
         <v>258</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B95" t="s">
         <v>259</v>
@@ -2453,7 +2453,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B96" t="s">
         <v>260</v>
@@ -2461,15 +2461,15 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B97" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B98" t="s">
         <v>261</v>
@@ -2477,7 +2477,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B99" t="s">
         <v>262</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B100" t="s">
         <v>263</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B101" t="s">
         <v>264</v>
@@ -2501,15 +2501,15 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B102" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B103" t="s">
         <v>265</v>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B104" t="s">
         <v>266</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B105" t="s">
         <v>267</v>
@@ -2533,7 +2533,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B106" t="s">
         <v>268</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B107" t="s">
         <v>269</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B108" t="s">
         <v>270</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B109" t="s">
         <v>271</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B110" t="s">
         <v>272</v>
@@ -2573,15 +2573,15 @@
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B111" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B112" t="s">
         <v>273</v>
@@ -2589,7 +2589,7 @@
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>275</v>
@@ -2597,7 +2597,7 @@
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>274</v>
@@ -2605,7 +2605,7 @@
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>276</v>
@@ -2613,7 +2613,7 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>277</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>278</v>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>279</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>280</v>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>281</v>
@@ -2653,7 +2653,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>282</v>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>283</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>284</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>285</v>
@@ -2685,23 +2685,23 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>286</v>
@@ -2709,7 +2709,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>287</v>
@@ -2717,95 +2717,95 @@
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B130" t="s">
-        <v>288</v>
+        <v>442</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B131" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B132" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B133" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B134" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B135" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B136" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B137" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B138" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B139" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B140" t="s">
         <v>98</v>
@@ -2813,39 +2813,39 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B141" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B142" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B143" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B144" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B145" t="s">
         <v>100</v>
@@ -2853,58 +2853,58 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B146" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B147" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B148" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B149" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B150" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B151" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B152" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -2917,8 +2917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C574"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4052,7 +4052,7 @@
         <v>chat_error_unknown_cmd</v>
       </c>
       <c r="B87" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C87" t="str">
         <f>IF(En!B87&lt;&gt;0,En!B87,"")</f>
@@ -4065,7 +4065,7 @@
         <v>chat_error</v>
       </c>
       <c r="B88" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C88" t="str">
         <f>IF(En!B88&lt;&gt;0,En!B88,"")</f>
@@ -4078,7 +4078,7 @@
         <v>chat_error_root</v>
       </c>
       <c r="B89" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C89" t="str">
         <f>IF(En!B89&lt;&gt;0,En!B89,"")</f>
@@ -4091,7 +4091,7 @@
         <v>chat_reply_contact</v>
       </c>
       <c r="B90" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C90" t="str">
         <f>IF(En!B90&lt;&gt;0,En!B90,"")</f>
@@ -4104,7 +4104,7 @@
         <v>chat_start_locating</v>
       </c>
       <c r="B91" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C91" t="str">
         <f>IF(En!B91&lt;&gt;0,En!B91,"")</f>
@@ -4117,7 +4117,7 @@
         <v>chat_start_ringing</v>
       </c>
       <c r="B92" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C92" t="str">
         <f>IF(En!B92&lt;&gt;0,En!B92,"")</f>
@@ -4130,7 +4130,7 @@
         <v>chat_error_ringing</v>
       </c>
       <c r="B93" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C93" t="str">
         <f>IF(En!B93&lt;&gt;0,En!B93,"")</f>
@@ -4143,7 +4143,7 @@
         <v>chat_stop_actions</v>
       </c>
       <c r="B94" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C94" t="str">
         <f>IF(En!B94&lt;&gt;0,En!B94,"")</f>
@@ -4156,7 +4156,7 @@
         <v>chat_send_sms</v>
       </c>
       <c r="B95" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C95" t="str">
         <f>IF(En!B95&lt;&gt;0,En!B95,"")</f>
@@ -4169,7 +4169,7 @@
         <v>chat_specify_details</v>
       </c>
       <c r="B96" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C96" t="str">
         <f>IF(En!B96&lt;&gt;0,En!B96,"")</f>
@@ -4182,7 +4182,7 @@
         <v>chat_no_match_for</v>
       </c>
       <c r="B97" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C97" t="str">
         <f>IF(En!B97&lt;&gt;0,En!B97,"")</f>
@@ -4195,7 +4195,7 @@
         <v>chat_mark_as_read</v>
       </c>
       <c r="B98" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C98" t="str">
         <f>IF(En!B98&lt;&gt;0,En!B98,"")</f>
@@ -4208,7 +4208,7 @@
         <v>chat_only_got_n_sms</v>
       </c>
       <c r="B99" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C99" t="str">
         <f>IF(En!B99&lt;&gt;0,En!B99,"")</f>
@@ -4221,7 +4221,7 @@
         <v>chat_no_sms</v>
       </c>
       <c r="B100" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C100" t="str">
         <f>IF(En!B100&lt;&gt;0,En!B100,"")</f>
@@ -4234,7 +4234,7 @@
         <v>chat_no_call</v>
       </c>
       <c r="B101" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C101" t="str">
         <f>IF(En!B101&lt;&gt;0,En!B101,"")</f>
@@ -4247,7 +4247,7 @@
         <v>chat_contact_found</v>
       </c>
       <c r="B102" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C102" t="str">
         <f>IF(En!B102&lt;&gt;0,En!B102,"")</f>
@@ -4260,7 +4260,7 @@
         <v>chat_phones</v>
       </c>
       <c r="B103" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C103" t="str">
         <f>IF(En!B103&lt;&gt;0,En!B103,"")</f>
@@ -4286,7 +4286,7 @@
         <v>chat_addresses</v>
       </c>
       <c r="B105" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C105" t="str">
         <f>IF(En!B105&lt;&gt;0,En!B105,"")</f>
@@ -4299,7 +4299,7 @@
         <v>chat_text_copied</v>
       </c>
       <c r="B106" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C106" t="str">
         <f>IF(En!B106&lt;&gt;0,En!B106,"")</f>
@@ -4312,7 +4312,7 @@
         <v>chat_error_clipboard</v>
       </c>
       <c r="B107" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C107" t="str">
         <f>IF(En!B107&lt;&gt;0,En!B107,"")</f>
@@ -4325,7 +4325,7 @@
         <v>chat_clipboard</v>
       </c>
       <c r="B108" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C108" t="str">
         <f>IF(En!B108&lt;&gt;0,En!B108,"")</f>
@@ -4338,7 +4338,7 @@
         <v>chat_choose_activity</v>
       </c>
       <c r="B109" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C109" t="str">
         <f>IF(En!B109&lt;&gt;0,En!B109,"")</f>
@@ -4351,7 +4351,7 @@
         <v>chat_dial</v>
       </c>
       <c r="B110" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C110" t="str">
         <f>IF(En!B110&lt;&gt;0,En!B110,"")</f>
@@ -4364,7 +4364,7 @@
         <v>chat_error_dial</v>
       </c>
       <c r="B111" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C111" t="str">
         <f>IF(En!B111&lt;&gt;0,En!B111,"")</f>
@@ -4377,7 +4377,7 @@
         <v>chat_help_title</v>
       </c>
       <c r="B112" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C112" t="str">
         <f>IF(En!B112&lt;&gt;0,En!B112,"")</f>
@@ -4390,7 +4390,7 @@
         <v>chat_help_help</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C113" t="str">
         <f>IF(En!B113&lt;&gt;0,En!B113,"")</f>
@@ -4403,7 +4403,7 @@
         <v>chat_help_stop</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C114" t="str">
         <f>IF(En!B114&lt;&gt;0,En!B114,"")</f>
@@ -4416,7 +4416,7 @@
         <v>chat_help_dial</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C115" t="str">
         <f>IF(En!B115&lt;&gt;0,En!B115,"")</f>
@@ -4429,7 +4429,7 @@
         <v>chat_help_sms_reply</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C116" t="str">
         <f>IF(En!B116&lt;&gt;0,En!B116,"")</f>
@@ -4442,7 +4442,7 @@
         <v>chat_help_sms_show_all</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C117" t="str">
         <f>IF(En!B117&lt;&gt;0,En!B117,"")</f>
@@ -4455,7 +4455,7 @@
         <v>chat_help_sms_show_contact</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C118" t="str">
         <f>IF(En!B118&lt;&gt;0,En!B118,"")</f>
@@ -4468,7 +4468,7 @@
         <v>chat_help_sms_send</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C119" t="str">
         <f>IF(En!B119&lt;&gt;0,En!B119,"")</f>
@@ -4481,7 +4481,7 @@
         <v>chat_help_mark_as_read</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C120" t="str">
         <f>IF(En!B120&lt;&gt;0,En!B120,"")</f>
@@ -4494,7 +4494,7 @@
         <v>chat_help_battery</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C121" t="str">
         <f>IF(En!B121&lt;&gt;0,En!B121,"")</f>
@@ -4507,7 +4507,7 @@
         <v>chat_help_calls</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C122" t="str">
         <f>IF(En!B122&lt;&gt;0,En!B122,"")</f>
@@ -4520,7 +4520,7 @@
         <v>chat_help_contact</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C123" t="str">
         <f>IF(En!B123&lt;&gt;0,En!B123,"")</f>
@@ -4533,7 +4533,7 @@
         <v>chat_help_geo</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C124" t="str">
         <f>IF(En!B124&lt;&gt;0,En!B124,"")</f>
@@ -4546,11 +4546,11 @@
         <v>chat_help_where</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>424</v>
+        <v>439</v>
       </c>
       <c r="C125" t="str">
         <f>IF(En!B125&lt;&gt;0,En!B125,"")</f>
-        <v>- %s: sends you google map updates about the location of the phone until you send \"stop\".</v>
+        <v>- %1$s: sends you google map updates about the location of the phone until you send %2$s.</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -4559,11 +4559,11 @@
         <v>chat_help_ring</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="C126" t="str">
         <f>IF(En!B126&lt;&gt;0,En!B126,"")</f>
-        <v>- %s: rings the phone until you send \"stop\".</v>
+        <v>- %1$s: rings the phone until you send %2$s.</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -4572,7 +4572,7 @@
         <v>chat_help_copy</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C127" t="str">
         <f>IF(En!B127&lt;&gt;0,En!B127,"")</f>
@@ -4585,7 +4585,7 @@
         <v>chat_help_cmd</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C128" t="str">
         <f>IF(En!B128&lt;&gt;0,En!B128,"")</f>
@@ -4598,7 +4598,7 @@
         <v>chat_help_write</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C129" t="str">
         <f>IF(En!B129&lt;&gt;0,En!B129,"")</f>
@@ -4611,11 +4611,11 @@
         <v>chat_help_urls</v>
       </c>
       <c r="B130" t="s">
-        <v>361</v>
+        <v>441</v>
       </c>
       <c r="C130" t="str">
         <f>IF(En!B130&lt;&gt;0,En!B130,"")</f>
-        <v>and you can paste links and open it with the appropriate application.</v>
+        <v>and you can paste %s links and open it with the appropriate application.</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -4624,7 +4624,7 @@
         <v>chat_call_unknown</v>
       </c>
       <c r="B131" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C131" t="str">
         <f>IF(En!B131&lt;&gt;0,En!B131,"")</f>
@@ -4637,7 +4637,7 @@
         <v>chat_call_incoming</v>
       </c>
       <c r="B132" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C132" t="str">
         <f>IF(En!B132&lt;&gt;0,En!B132,"")</f>
@@ -4650,7 +4650,7 @@
         <v>chat_call_outgoing</v>
       </c>
       <c r="B133" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C133" t="str">
         <f>IF(En!B133&lt;&gt;0,En!B133,"")</f>
@@ -4663,7 +4663,7 @@
         <v>chat_call_missed</v>
       </c>
       <c r="B134" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C134" t="str">
         <f>IF(En!B134&lt;&gt;0,En!B134,"")</f>
@@ -4676,7 +4676,7 @@
         <v>chat_call_duration</v>
       </c>
       <c r="B135" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="C135" t="str">
         <f>IF(En!B135&lt;&gt;0,En!B135,"")</f>
@@ -4689,7 +4689,7 @@
         <v>chat_welcome</v>
       </c>
       <c r="B136" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C136" t="str">
         <f>IF(En!B136&lt;&gt;0,En!B136,"")</f>
@@ -4702,7 +4702,7 @@
         <v>chat_app_stop</v>
       </c>
       <c r="B137" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C137" t="str">
         <f>IF(En!B137&lt;&gt;0,En!B137,"")</f>
@@ -4715,7 +4715,7 @@
         <v>chat_is_calling</v>
       </c>
       <c r="B138" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C138" t="str">
         <f>IF(En!B138&lt;&gt;0,En!B138,"")</f>
@@ -4728,7 +4728,7 @@
         <v>chat_call_hidden</v>
       </c>
       <c r="B139" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C139" t="str">
         <f>IF(En!B139&lt;&gt;0,En!B139,"")</f>
@@ -4741,7 +4741,7 @@
         <v>chat_sms_sent</v>
       </c>
       <c r="B140" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C140" t="str">
         <f>IF(En!B140&lt;&gt;0,En!B140,"")</f>
@@ -4754,7 +4754,7 @@
         <v>chat_sms_failure</v>
       </c>
       <c r="B141" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C141" t="str">
         <f>IF(En!B141&lt;&gt;0,En!B141,"")</f>
@@ -4767,7 +4767,7 @@
         <v>chat_sms_no_service</v>
       </c>
       <c r="B142" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C142" t="str">
         <f>IF(En!B142&lt;&gt;0,En!B142,"")</f>
@@ -4780,7 +4780,7 @@
         <v>chat_sms_null_pdu</v>
       </c>
       <c r="B143" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C143" t="str">
         <f>IF(En!B143&lt;&gt;0,En!B143,"")</f>
@@ -4793,7 +4793,7 @@
         <v>chat_sms_radio_off</v>
       </c>
       <c r="B144" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C144" t="str">
         <f>IF(En!B144&lt;&gt;0,En!B144,"")</f>
@@ -4806,7 +4806,7 @@
         <v>chat_sms_delivered</v>
       </c>
       <c r="B145" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C145" t="str">
         <f>IF(En!B145&lt;&gt;0,En!B145,"")</f>
@@ -4819,7 +4819,7 @@
         <v>chat_sms_not_delivered</v>
       </c>
       <c r="B146" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C146" t="str">
         <f>IF(En!B146&lt;&gt;0,En!B146,"")</f>
@@ -4832,7 +4832,7 @@
         <v>chat_log_failed</v>
       </c>
       <c r="B147" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C147" t="str">
         <f>IF(En!B147&lt;&gt;0,En!B147,"")</f>
@@ -4845,7 +4845,7 @@
         <v>chat_log_unavailable</v>
       </c>
       <c r="B148" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C148" t="str">
         <f>IF(En!B148&lt;&gt;0,En!B148,"")</f>
@@ -4858,7 +4858,7 @@
         <v>chat_geo_accuracy</v>
       </c>
       <c r="B149" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C149" t="str">
         <f>IF(En!B149&lt;&gt;0,En!B149,"")</f>
@@ -4871,7 +4871,7 @@
         <v>chat_geo_altitude</v>
       </c>
       <c r="B150" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="C150" t="str">
         <f>IF(En!B150&lt;&gt;0,En!B150,"")</f>
@@ -4884,7 +4884,7 @@
         <v>chat_geo_speed</v>
       </c>
       <c r="B151" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="C151" t="str">
         <f>IF(En!B151&lt;&gt;0,En!B151,"")</f>
@@ -4897,7 +4897,7 @@
         <v>chat_geo_provider</v>
       </c>
       <c r="B152" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C152" t="str">
         <f>IF(En!B152&lt;&gt;0,En!B152,"")</f>
@@ -11649,7 +11649,7 @@
       </c>
       <c r="D125" t="str">
         <f>IF(En!B125&lt;&gt;0,En!B125,"")</f>
-        <v>- %s: sends you google map updates about the location of the phone until you send \"stop\".</v>
+        <v>- %1$s: sends you google map updates about the location of the phone until you send %2$s.</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="5"/>
@@ -11671,7 +11671,7 @@
       </c>
       <c r="D126" t="str">
         <f>IF(En!B126&lt;&gt;0,En!B126,"")</f>
-        <v>- %s: rings the phone until you send \"stop\".</v>
+        <v>- %1$s: rings the phone until you send %2$s.</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="5"/>
@@ -11759,7 +11759,7 @@
       </c>
       <c r="D130" t="str">
         <f>IF(En!B130&lt;&gt;0,En!B130,"")</f>
-        <v>and you can paste links and open it with the appropriate application.</v>
+        <v>and you can paste %s links and open it with the appropriate application.</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" ref="E130:E193" si="8">IF(B130&lt;&gt;"","&lt;/string&gt;","")</f>
@@ -19783,8 +19783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E480"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22539,7 +22539,7 @@
       </c>
       <c r="D125" t="str">
         <f>IF(Fr!B125&lt;&gt;0,Fr!B125,"")</f>
-        <v>- %s: envoie continue de liens Gmap pour localiser le téléphone jusqu\'à l\'envoie de la commande \"stop\".</v>
+        <v>- %1$s: envoie continue de liens Gmap pour localiser le téléphone jusqu\'à l\'envoie de la commande %2$s.</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="5"/>
@@ -22561,7 +22561,7 @@
       </c>
       <c r="D126" t="str">
         <f>IF(Fr!B126&lt;&gt;0,Fr!B126,"")</f>
-        <v>- %s: faire sonner le téléphone jusqu\'à l\'envoie de la commande \"stop\".</v>
+        <v>- %1$s: faire sonner le téléphone jusqu\'à l\'envoie de la commande %2$s.</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="5"/>
@@ -22649,7 +22649,7 @@
       </c>
       <c r="D130" t="str">
         <f>IF(Fr!B130&lt;&gt;0,Fr!B130,"")</f>
-        <v>et coller les liens http pour les ouvrir dans le navigateur du téléphone.</v>
+        <v>et coller les liens %s pour les ouvrir dans le navigateur du téléphone.</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" ref="E130:E193" si="8">IF(B130&lt;&gt;"","&lt;/string&gt;","")</f>

</xml_diff>

<commit_message>
Remove values-en because default values are in english Remove untranlated string arrays in localized array.xml Update translations.xlsx Update local without restart application
</commit_message>
<xml_diff>
--- a/Translations.xlsx
+++ b/Translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="20055" windowHeight="12015"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="20055" windowHeight="12015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="En" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="594">
   <si>
     <t>pref_app</t>
   </si>
@@ -1777,6 +1777,30 @@
   </si>
   <si>
     <t>Can\'t have root access!</t>
+  </si>
+  <si>
+    <t>pref_app_locale</t>
+  </si>
+  <si>
+    <t>pref_app_locale_help</t>
+  </si>
+  <si>
+    <t>Choose the application localization</t>
+  </si>
+  <si>
+    <t>Localization</t>
+  </si>
+  <si>
+    <t>Choisir la langue</t>
+  </si>
+  <si>
+    <t>Langue</t>
+  </si>
+  <si>
+    <t>Sprache</t>
+  </si>
+  <si>
+    <t>Sprachumgebung der Anwendung festlegen</t>
   </si>
 </sst>
 </file>
@@ -2109,10 +2133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B152"/>
+  <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3338,6 +3362,22 @@
         <v>396</v>
       </c>
     </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>586</v>
+      </c>
+      <c r="B153" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>587</v>
+      </c>
+      <c r="B154" t="s">
+        <v>589</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3348,8 +3388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C574"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5338,21 +5378,27 @@
     <row r="153" spans="1:3">
       <c r="A153" t="str">
         <f>IF(En!A153&lt;&gt;0,En!A153,"")</f>
-        <v/>
+        <v>pref_app_locale</v>
+      </c>
+      <c r="B153" t="s">
+        <v>590</v>
       </c>
       <c r="C153" t="str">
         <f>IF(En!B153&lt;&gt;0,En!B153,"")</f>
-        <v/>
+        <v>Choose the application localization</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="str">
         <f>IF(En!A154&lt;&gt;0,En!A154,"")</f>
-        <v/>
+        <v>pref_app_locale_help</v>
+      </c>
+      <c r="B154" t="s">
+        <v>591</v>
       </c>
       <c r="C154" t="str">
         <f>IF(En!B154&lt;&gt;0,En!B154,"")</f>
-        <v/>
+        <v>Localization</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -9324,8 +9370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C574"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11314,21 +11360,27 @@
     <row r="153" spans="1:3">
       <c r="A153" t="str">
         <f>IF(En!A153&lt;&gt;0,En!A153,"")</f>
-        <v/>
+        <v>pref_app_locale</v>
+      </c>
+      <c r="B153" t="s">
+        <v>592</v>
       </c>
       <c r="C153" t="str">
         <f>IF(En!B153&lt;&gt;0,En!B153,"")</f>
-        <v/>
+        <v>Choose the application localization</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="str">
         <f>IF(En!A154&lt;&gt;0,En!A154,"")</f>
-        <v/>
+        <v>pref_app_locale_help</v>
+      </c>
+      <c r="B154" t="s">
+        <v>593</v>
       </c>
       <c r="C154" t="str">
         <f>IF(En!B154&lt;&gt;0,En!B154,"")</f>
-        <v/>
+        <v>Localization</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -18660,45 +18712,45 @@
     <row r="153" spans="1:5">
       <c r="A153" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v xml:space="preserve">    &lt;string name="</v>
       </c>
       <c r="B153" t="str">
         <f>IF(En!A153&lt;&gt;0,En!A153,"")</f>
-        <v/>
+        <v>pref_app_locale</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>"&gt;</v>
       </c>
       <c r="D153" t="str">
         <f>IF(En!B153&lt;&gt;0,En!B153,"")</f>
-        <v/>
+        <v>Choose the application localization</v>
       </c>
       <c r="E153" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>&lt;/string&gt;</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v xml:space="preserve">    &lt;string name="</v>
       </c>
       <c r="B154" t="str">
         <f>IF(En!A154&lt;&gt;0,En!A154,"")</f>
-        <v/>
+        <v>pref_app_locale_help</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>"&gt;</v>
       </c>
       <c r="D154" t="str">
         <f>IF(En!B154&lt;&gt;0,En!B154,"")</f>
-        <v/>
+        <v>Localization</v>
       </c>
       <c r="E154" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>&lt;/string&gt;</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -29550,45 +29602,45 @@
     <row r="153" spans="1:5">
       <c r="A153" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v xml:space="preserve">    &lt;string name="</v>
       </c>
       <c r="B153" t="str">
         <f>IF(Fr!A153&lt;&gt;0,Fr!A153,"")</f>
-        <v/>
+        <v>pref_app_locale</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>"&gt;</v>
       </c>
       <c r="D153" t="str">
         <f>IF(Fr!B153&lt;&gt;0,Fr!B153,"")</f>
-        <v/>
+        <v>Choisir la langue</v>
       </c>
       <c r="E153" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>&lt;/string&gt;</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v xml:space="preserve">    &lt;string name="</v>
       </c>
       <c r="B154" t="str">
         <f>IF(Fr!A154&lt;&gt;0,Fr!A154,"")</f>
-        <v/>
+        <v>pref_app_locale_help</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>"&gt;</v>
       </c>
       <c r="D154" t="str">
         <f>IF(Fr!B154&lt;&gt;0,Fr!B154,"")</f>
-        <v/>
+        <v>Langue</v>
       </c>
       <c r="E154" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>&lt;/string&gt;</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -40132,45 +40184,45 @@
     <row r="153" spans="1:5">
       <c r="A153" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v xml:space="preserve">    &lt;string name="</v>
       </c>
       <c r="B153" t="str">
         <f>IF(De!A153&lt;&gt;0,De!A153,"")</f>
-        <v/>
+        <v>pref_app_locale</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>"&gt;</v>
       </c>
       <c r="D153" t="str">
         <f>IF(De!B153&lt;&gt;0,De!B153,"")</f>
-        <v/>
+        <v>Sprache</v>
       </c>
       <c r="E153" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>&lt;/string&gt;</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v xml:space="preserve">    &lt;string name="</v>
       </c>
       <c r="B154" t="str">
         <f>IF(De!A154&lt;&gt;0,De!A154,"")</f>
-        <v/>
+        <v>pref_app_locale_help</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>"&gt;</v>
       </c>
       <c r="D154" t="str">
         <f>IF(De!B154&lt;&gt;0,De!B154,"")</f>
-        <v/>
+        <v>Sprachumgebung der Anwendung festlegen</v>
       </c>
       <c r="E154" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>&lt;/string&gt;</v>
       </c>
     </row>
     <row r="155" spans="1:5">

</xml_diff>

<commit_message>
Add smack javadoc into project Fix some translation issues Fix chat room's multiple message notification issue by changing xmpp server
</commit_message>
<xml_diff>
--- a/Translations.xlsx
+++ b/Translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="20055" windowHeight="12015" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="20055" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="En" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="596">
   <si>
     <t>pref_app</t>
   </si>
@@ -798,21 +798,9 @@
     <t>Stopping ongoing actions</t>
   </si>
   <si>
-    <t>Sending sms to %s</t>
-  </si>
-  <si>
     <t>Specify more details:</t>
   </si>
   <si>
-    <t>Mark %s\'s sms as read</t>
-  </si>
-  <si>
-    <t>Only got %d sms</t>
-  </si>
-  <si>
-    <t>No sms found</t>
-  </si>
-  <si>
     <t>No phone call found</t>
   </si>
   <si>
@@ -852,21 +840,6 @@
     <t>- %s: dial the specified contact.</t>
   </si>
   <si>
-    <t>- %s: send a sms to your last recipient with content message.</t>
-  </si>
-  <si>
-    <t>- %s: display last sent sms from all contact.</t>
-  </si>
-  <si>
-    <t>- %s: display last sent sms from searched contacts.</t>
-  </si>
-  <si>
-    <t>- %s: sends a sms to number with content message.</t>
-  </si>
-  <si>
-    <t>- %1$s or %2$s: mark sms as read for last recipient or given contact.</t>
-  </si>
-  <si>
     <t>- %1$s or %2$s: show battery level in percent.</t>
   </si>
   <si>
@@ -1386,9 +1359,6 @@
     <t>Anzahl der SMS</t>
   </si>
   <si>
-    <t xml:space="preserve">Anzahl der SMS gezeigt werden </t>
-  </si>
-  <si>
     <t>Zeige gesendete SMS</t>
   </si>
   <si>
@@ -1404,9 +1374,6 @@
     <t>Klingelton</t>
   </si>
   <si>
-    <t>Klingelton der durch den ring Befehl abgespielt wird</t>
-  </si>
-  <si>
     <t>Verbindungseinstellungen</t>
   </si>
   <si>
@@ -1452,9 +1419,6 @@
     <t>Service Name (rechte Teil der JID)</t>
   </si>
   <si>
-    <t>Benachrichtigungseinstellungen</t>
-  </si>
-  <si>
     <t>Bei erfolgreicher Verbindung</t>
   </si>
   <si>
@@ -1530,9 +1494,6 @@
     <t>Trenne...</t>
   </si>
   <si>
-    <t>Warte...</t>
-  </si>
-  <si>
     <t>Warte auf Verbindung...</t>
   </si>
   <si>
@@ -1801,6 +1762,51 @@
   </si>
   <si>
     <t>Sprachumgebung der Anwendung festlegen</t>
+  </si>
+  <si>
+    <t>Anzahl der SMS die ausgegeben werden</t>
+  </si>
+  <si>
+    <t>Klingelton der durch den \"ring\" Befehl abgespielt wird</t>
+  </si>
+  <si>
+    <t>Verbindungsoptionen</t>
+  </si>
+  <si>
+    <t>Benachrichtigungsoptionen</t>
+  </si>
+  <si>
+    <t>Anwendungsoptionen</t>
+  </si>
+  <si>
+    <t>Wartend...</t>
+  </si>
+  <si>
+    <t>Sending SMS to %s</t>
+  </si>
+  <si>
+    <t>Mark %s\'s SMS as read</t>
+  </si>
+  <si>
+    <t>Only got %d SMS</t>
+  </si>
+  <si>
+    <t>No SMS found</t>
+  </si>
+  <si>
+    <t>- %s: send a SMS to your last recipient with content message.</t>
+  </si>
+  <si>
+    <t>- %s: display last sent SMS from all contact.</t>
+  </si>
+  <si>
+    <t>- %s: display last sent SMS from searched contacts.</t>
+  </si>
+  <si>
+    <t>- %s: sends a SMS to number with content message.</t>
+  </si>
+  <si>
+    <t>- %1$s or %2$s: mark SMS as read for last recipient or given contact.</t>
   </si>
 </sst>
 </file>
@@ -2135,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="B157" sqref="B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2839,7 +2845,7 @@
         <v>247</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2855,7 +2861,7 @@
         <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2868,7 +2874,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B91" t="s">
         <v>255</v>
@@ -2876,7 +2882,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B92" t="s">
         <v>256</v>
@@ -2884,7 +2890,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B93" t="s">
         <v>257</v>
@@ -2892,7 +2898,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B94" t="s">
         <v>258</v>
@@ -2900,367 +2906,367 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B95" t="s">
-        <v>259</v>
+        <v>587</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B97" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B98" t="s">
-        <v>261</v>
+        <v>588</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B99" t="s">
-        <v>262</v>
+        <v>589</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B100" t="s">
-        <v>263</v>
+        <v>590</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B101" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B102" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B103" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B104" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B105" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B106" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B107" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B108" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B109" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B110" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B111" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="B112" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>277</v>
+        <v>591</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>278</v>
+        <v>592</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>279</v>
+        <v>593</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>280</v>
+        <v>594</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>281</v>
+        <v>595</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B130" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B131" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B132" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B133" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="B134" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B135" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B136" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B137" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B138" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="B139" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B140" t="s">
         <v>98</v>
@@ -3268,39 +3274,39 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B141" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B142" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="B143" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B144" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="B145" t="s">
         <v>100</v>
@@ -3308,74 +3314,74 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="B146" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="B147" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B148" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="B149" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="B150" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="B151" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="B152" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="B153" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="B154" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -3388,7 +3394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C574"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
@@ -4523,7 +4529,7 @@
         <v>chat_error_unknown_cmd</v>
       </c>
       <c r="B87" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="C87" t="str">
         <f>IF(En!B87&lt;&gt;0,En!B87,"")</f>
@@ -4536,7 +4542,7 @@
         <v>chat_error</v>
       </c>
       <c r="B88" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C88" t="str">
         <f>IF(En!B88&lt;&gt;0,En!B88,"")</f>
@@ -4549,7 +4555,7 @@
         <v>chat_error_root</v>
       </c>
       <c r="B89" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C89" t="str">
         <f>IF(En!B89&lt;&gt;0,En!B89,"")</f>
@@ -4562,7 +4568,7 @@
         <v>chat_reply_contact</v>
       </c>
       <c r="B90" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C90" t="str">
         <f>IF(En!B90&lt;&gt;0,En!B90,"")</f>
@@ -4575,7 +4581,7 @@
         <v>chat_start_locating</v>
       </c>
       <c r="B91" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C91" t="str">
         <f>IF(En!B91&lt;&gt;0,En!B91,"")</f>
@@ -4588,7 +4594,7 @@
         <v>chat_start_ringing</v>
       </c>
       <c r="B92" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C92" t="str">
         <f>IF(En!B92&lt;&gt;0,En!B92,"")</f>
@@ -4601,7 +4607,7 @@
         <v>chat_error_ringing</v>
       </c>
       <c r="B93" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C93" t="str">
         <f>IF(En!B93&lt;&gt;0,En!B93,"")</f>
@@ -4614,7 +4620,7 @@
         <v>chat_stop_actions</v>
       </c>
       <c r="B94" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C94" t="str">
         <f>IF(En!B94&lt;&gt;0,En!B94,"")</f>
@@ -4627,11 +4633,11 @@
         <v>chat_send_sms</v>
       </c>
       <c r="B95" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C95" t="str">
         <f>IF(En!B95&lt;&gt;0,En!B95,"")</f>
-        <v>Sending sms to %s</v>
+        <v>Sending SMS to %s</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -4640,7 +4646,7 @@
         <v>chat_specify_details</v>
       </c>
       <c r="B96" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C96" t="str">
         <f>IF(En!B96&lt;&gt;0,En!B96,"")</f>
@@ -4653,7 +4659,7 @@
         <v>chat_no_match_for</v>
       </c>
       <c r="B97" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="C97" t="str">
         <f>IF(En!B97&lt;&gt;0,En!B97,"")</f>
@@ -4666,11 +4672,11 @@
         <v>chat_mark_as_read</v>
       </c>
       <c r="B98" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C98" t="str">
         <f>IF(En!B98&lt;&gt;0,En!B98,"")</f>
-        <v>Mark %s\'s sms as read</v>
+        <v>Mark %s\'s SMS as read</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -4679,11 +4685,11 @@
         <v>chat_only_got_n_sms</v>
       </c>
       <c r="B99" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C99" t="str">
         <f>IF(En!B99&lt;&gt;0,En!B99,"")</f>
-        <v>Only got %d sms</v>
+        <v>Only got %d SMS</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -4692,11 +4698,11 @@
         <v>chat_no_sms</v>
       </c>
       <c r="B100" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="C100" t="str">
         <f>IF(En!B100&lt;&gt;0,En!B100,"")</f>
-        <v>No sms found</v>
+        <v>No SMS found</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -4705,7 +4711,7 @@
         <v>chat_no_call</v>
       </c>
       <c r="B101" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C101" t="str">
         <f>IF(En!B101&lt;&gt;0,En!B101,"")</f>
@@ -4718,7 +4724,7 @@
         <v>chat_contact_found</v>
       </c>
       <c r="B102" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C102" t="str">
         <f>IF(En!B102&lt;&gt;0,En!B102,"")</f>
@@ -4731,7 +4737,7 @@
         <v>chat_phones</v>
       </c>
       <c r="B103" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C103" t="str">
         <f>IF(En!B103&lt;&gt;0,En!B103,"")</f>
@@ -4744,7 +4750,7 @@
         <v>chat_emails</v>
       </c>
       <c r="B104" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C104" t="str">
         <f>IF(En!B104&lt;&gt;0,En!B104,"")</f>
@@ -4757,7 +4763,7 @@
         <v>chat_addresses</v>
       </c>
       <c r="B105" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C105" t="str">
         <f>IF(En!B105&lt;&gt;0,En!B105,"")</f>
@@ -4770,7 +4776,7 @@
         <v>chat_text_copied</v>
       </c>
       <c r="B106" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C106" t="str">
         <f>IF(En!B106&lt;&gt;0,En!B106,"")</f>
@@ -4783,7 +4789,7 @@
         <v>chat_error_clipboard</v>
       </c>
       <c r="B107" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C107" t="str">
         <f>IF(En!B107&lt;&gt;0,En!B107,"")</f>
@@ -4796,7 +4802,7 @@
         <v>chat_clipboard</v>
       </c>
       <c r="B108" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C108" t="str">
         <f>IF(En!B108&lt;&gt;0,En!B108,"")</f>
@@ -4809,7 +4815,7 @@
         <v>chat_choose_activity</v>
       </c>
       <c r="B109" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="C109" t="str">
         <f>IF(En!B109&lt;&gt;0,En!B109,"")</f>
@@ -4822,7 +4828,7 @@
         <v>chat_dial</v>
       </c>
       <c r="B110" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C110" t="str">
         <f>IF(En!B110&lt;&gt;0,En!B110,"")</f>
@@ -4835,7 +4841,7 @@
         <v>chat_error_dial</v>
       </c>
       <c r="B111" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C111" t="str">
         <f>IF(En!B111&lt;&gt;0,En!B111,"")</f>
@@ -4848,7 +4854,7 @@
         <v>chat_help_title</v>
       </c>
       <c r="B112" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C112" t="str">
         <f>IF(En!B112&lt;&gt;0,En!B112,"")</f>
@@ -4861,7 +4867,7 @@
         <v>chat_help_help</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C113" t="str">
         <f>IF(En!B113&lt;&gt;0,En!B113,"")</f>
@@ -4874,7 +4880,7 @@
         <v>chat_help_stop</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C114" t="str">
         <f>IF(En!B114&lt;&gt;0,En!B114,"")</f>
@@ -4887,7 +4893,7 @@
         <v>chat_help_dial</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="C115" t="str">
         <f>IF(En!B115&lt;&gt;0,En!B115,"")</f>
@@ -4900,11 +4906,11 @@
         <v>chat_help_sms_reply</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C116" t="str">
         <f>IF(En!B116&lt;&gt;0,En!B116,"")</f>
-        <v>- %s: send a sms to your last recipient with content message.</v>
+        <v>- %s: send a SMS to your last recipient with content message.</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -4913,11 +4919,11 @@
         <v>chat_help_sms_show_all</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C117" t="str">
         <f>IF(En!B117&lt;&gt;0,En!B117,"")</f>
-        <v>- %s: display last sent sms from all contact.</v>
+        <v>- %s: display last sent SMS from all contact.</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -4926,11 +4932,11 @@
         <v>chat_help_sms_show_contact</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="C118" t="str">
         <f>IF(En!B118&lt;&gt;0,En!B118,"")</f>
-        <v>- %s: display last sent sms from searched contacts.</v>
+        <v>- %s: display last sent SMS from searched contacts.</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -4939,11 +4945,11 @@
         <v>chat_help_sms_send</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="C119" t="str">
         <f>IF(En!B119&lt;&gt;0,En!B119,"")</f>
-        <v>- %s: sends a sms to number with content message.</v>
+        <v>- %s: sends a SMS to number with content message.</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -4952,11 +4958,11 @@
         <v>chat_help_mark_as_read</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C120" t="str">
         <f>IF(En!B120&lt;&gt;0,En!B120,"")</f>
-        <v>- %1$s or %2$s: mark sms as read for last recipient or given contact.</v>
+        <v>- %1$s or %2$s: mark SMS as read for last recipient or given contact.</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -4965,7 +4971,7 @@
         <v>chat_help_battery</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C121" t="str">
         <f>IF(En!B121&lt;&gt;0,En!B121,"")</f>
@@ -4978,7 +4984,7 @@
         <v>chat_help_calls</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="C122" t="str">
         <f>IF(En!B122&lt;&gt;0,En!B122,"")</f>
@@ -4991,7 +4997,7 @@
         <v>chat_help_contact</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C123" t="str">
         <f>IF(En!B123&lt;&gt;0,En!B123,"")</f>
@@ -5004,7 +5010,7 @@
         <v>chat_help_geo</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C124" t="str">
         <f>IF(En!B124&lt;&gt;0,En!B124,"")</f>
@@ -5017,7 +5023,7 @@
         <v>chat_help_where</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="C125" t="str">
         <f>IF(En!B125&lt;&gt;0,En!B125,"")</f>
@@ -5030,7 +5036,7 @@
         <v>chat_help_ring</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="C126" t="str">
         <f>IF(En!B126&lt;&gt;0,En!B126,"")</f>
@@ -5043,7 +5049,7 @@
         <v>chat_help_copy</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C127" t="str">
         <f>IF(En!B127&lt;&gt;0,En!B127,"")</f>
@@ -5056,7 +5062,7 @@
         <v>chat_help_cmd</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="C128" t="str">
         <f>IF(En!B128&lt;&gt;0,En!B128,"")</f>
@@ -5069,7 +5075,7 @@
         <v>chat_help_write</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="C129" t="str">
         <f>IF(En!B129&lt;&gt;0,En!B129,"")</f>
@@ -5082,7 +5088,7 @@
         <v>chat_help_urls</v>
       </c>
       <c r="B130" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="C130" t="str">
         <f>IF(En!B130&lt;&gt;0,En!B130,"")</f>
@@ -5095,7 +5101,7 @@
         <v>chat_call_unknown</v>
       </c>
       <c r="B131" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C131" t="str">
         <f>IF(En!B131&lt;&gt;0,En!B131,"")</f>
@@ -5108,7 +5114,7 @@
         <v>chat_call_incoming</v>
       </c>
       <c r="B132" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C132" t="str">
         <f>IF(En!B132&lt;&gt;0,En!B132,"")</f>
@@ -5121,7 +5127,7 @@
         <v>chat_call_outgoing</v>
       </c>
       <c r="B133" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="C133" t="str">
         <f>IF(En!B133&lt;&gt;0,En!B133,"")</f>
@@ -5134,7 +5140,7 @@
         <v>chat_call_missed</v>
       </c>
       <c r="B134" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C134" t="str">
         <f>IF(En!B134&lt;&gt;0,En!B134,"")</f>
@@ -5147,7 +5153,7 @@
         <v>chat_call_duration</v>
       </c>
       <c r="B135" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="C135" t="str">
         <f>IF(En!B135&lt;&gt;0,En!B135,"")</f>
@@ -5160,7 +5166,7 @@
         <v>chat_welcome</v>
       </c>
       <c r="B136" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="C136" t="str">
         <f>IF(En!B136&lt;&gt;0,En!B136,"")</f>
@@ -5173,7 +5179,7 @@
         <v>chat_app_stop</v>
       </c>
       <c r="B137" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="C137" t="str">
         <f>IF(En!B137&lt;&gt;0,En!B137,"")</f>
@@ -5186,7 +5192,7 @@
         <v>chat_is_calling</v>
       </c>
       <c r="B138" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="C138" t="str">
         <f>IF(En!B138&lt;&gt;0,En!B138,"")</f>
@@ -5199,7 +5205,7 @@
         <v>chat_call_hidden</v>
       </c>
       <c r="B139" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="C139" t="str">
         <f>IF(En!B139&lt;&gt;0,En!B139,"")</f>
@@ -5212,7 +5218,7 @@
         <v>chat_sms_sent</v>
       </c>
       <c r="B140" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C140" t="str">
         <f>IF(En!B140&lt;&gt;0,En!B140,"")</f>
@@ -5225,7 +5231,7 @@
         <v>chat_sms_failure</v>
       </c>
       <c r="B141" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="C141" t="str">
         <f>IF(En!B141&lt;&gt;0,En!B141,"")</f>
@@ -5238,7 +5244,7 @@
         <v>chat_sms_no_service</v>
       </c>
       <c r="B142" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C142" t="str">
         <f>IF(En!B142&lt;&gt;0,En!B142,"")</f>
@@ -5251,7 +5257,7 @@
         <v>chat_sms_null_pdu</v>
       </c>
       <c r="B143" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="C143" t="str">
         <f>IF(En!B143&lt;&gt;0,En!B143,"")</f>
@@ -5264,7 +5270,7 @@
         <v>chat_sms_radio_off</v>
       </c>
       <c r="B144" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="C144" t="str">
         <f>IF(En!B144&lt;&gt;0,En!B144,"")</f>
@@ -5277,7 +5283,7 @@
         <v>chat_sms_delivered</v>
       </c>
       <c r="B145" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="C145" t="str">
         <f>IF(En!B145&lt;&gt;0,En!B145,"")</f>
@@ -5290,7 +5296,7 @@
         <v>chat_sms_not_delivered</v>
       </c>
       <c r="B146" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C146" t="str">
         <f>IF(En!B146&lt;&gt;0,En!B146,"")</f>
@@ -5303,7 +5309,7 @@
         <v>chat_log_failed</v>
       </c>
       <c r="B147" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="C147" t="str">
         <f>IF(En!B147&lt;&gt;0,En!B147,"")</f>
@@ -5316,7 +5322,7 @@
         <v>chat_log_unavailable</v>
       </c>
       <c r="B148" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C148" t="str">
         <f>IF(En!B148&lt;&gt;0,En!B148,"")</f>
@@ -5329,7 +5335,7 @@
         <v>chat_geo_accuracy</v>
       </c>
       <c r="B149" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="C149" t="str">
         <f>IF(En!B149&lt;&gt;0,En!B149,"")</f>
@@ -5342,7 +5348,7 @@
         <v>chat_geo_altitude</v>
       </c>
       <c r="B150" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="C150" t="str">
         <f>IF(En!B150&lt;&gt;0,En!B150,"")</f>
@@ -5355,7 +5361,7 @@
         <v>chat_geo_speed</v>
       </c>
       <c r="B151" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="C151" t="str">
         <f>IF(En!B151&lt;&gt;0,En!B151,"")</f>
@@ -5368,7 +5374,7 @@
         <v>chat_geo_provider</v>
       </c>
       <c r="B152" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="C152" t="str">
         <f>IF(En!B152&lt;&gt;0,En!B152,"")</f>
@@ -5381,7 +5387,7 @@
         <v>pref_app_locale</v>
       </c>
       <c r="B153" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="C153" t="str">
         <f>IF(En!B153&lt;&gt;0,En!B153,"")</f>
@@ -5394,7 +5400,7 @@
         <v>pref_app_locale_help</v>
       </c>
       <c r="B154" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="C154" t="str">
         <f>IF(En!B154&lt;&gt;0,En!B154,"")</f>
@@ -9370,8 +9376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9387,7 +9393,7 @@
         <v>pref_app</v>
       </c>
       <c r="B1" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="C1" t="str">
         <f>IF(En!B1&lt;&gt;0,En!B1,"")</f>
@@ -9400,7 +9406,7 @@
         <v>pref_app_auto_start_options</v>
       </c>
       <c r="B2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="C2" t="str">
         <f>IF(En!B2&lt;&gt;0,En!B2,"")</f>
@@ -9413,7 +9419,7 @@
         <v>pref_app_auto_stop_options</v>
       </c>
       <c r="B3" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="C3" t="str">
         <f>IF(En!B3&lt;&gt;0,En!B3,"")</f>
@@ -9426,7 +9432,7 @@
         <v>pref_app_start_at_boot</v>
       </c>
       <c r="B4" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="C4" t="str">
         <f>IF(En!B4&lt;&gt;0,En!B4,"")</f>
@@ -9439,7 +9445,7 @@
         <v>pref_app_start_at_boot_help</v>
       </c>
       <c r="B5" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="C5" t="str">
         <f>IF(En!B5&lt;&gt;0,En!B5,"")</f>
@@ -9452,7 +9458,7 @@
         <v>pref_app_start_on_power_connected</v>
       </c>
       <c r="B6" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="C6" t="str">
         <f>IF(En!B6&lt;&gt;0,En!B6,"")</f>
@@ -9465,7 +9471,7 @@
         <v>pref_app_start_on_power_connected_help</v>
       </c>
       <c r="B7" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="C7" t="str">
         <f>IF(En!B7&lt;&gt;0,En!B7,"")</f>
@@ -9478,7 +9484,7 @@
         <v>pref_app_stop_on_power_disconnected</v>
       </c>
       <c r="B8" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="C8" t="str">
         <f>IF(En!B8&lt;&gt;0,En!B8,"")</f>
@@ -9491,7 +9497,7 @@
         <v>pref_app_stop_on_power_disconnected_help</v>
       </c>
       <c r="B9" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="C9" t="str">
         <f>IF(En!B9&lt;&gt;0,En!B9,"")</f>
@@ -9504,7 +9510,7 @@
         <v>pref_app_show_status_icon</v>
       </c>
       <c r="B10" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="C10" t="str">
         <f>IF(En!B10&lt;&gt;0,En!B10,"")</f>
@@ -9517,7 +9523,7 @@
         <v>pref_app_show_status_icon_help</v>
       </c>
       <c r="B11" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="C11" t="str">
         <f>IF(En!B11&lt;&gt;0,En!B11,"")</f>
@@ -9530,7 +9536,7 @@
         <v>pref_app_format_responses</v>
       </c>
       <c r="B12" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="C12" t="str">
         <f>IF(En!B12&lt;&gt;0,En!B12,"")</f>
@@ -9543,7 +9549,7 @@
         <v>pref_app_format_responses_help</v>
       </c>
       <c r="B13" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="C13" t="str">
         <f>IF(En!B13&lt;&gt;0,En!B13,"")</f>
@@ -9556,7 +9562,7 @@
         <v>pref_app_sms_number</v>
       </c>
       <c r="B14" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="C14" t="str">
         <f>IF(En!B14&lt;&gt;0,En!B14,"")</f>
@@ -9569,7 +9575,7 @@
         <v>pref_app_sms_number_help</v>
       </c>
       <c r="B15" t="s">
-        <v>455</v>
+        <v>581</v>
       </c>
       <c r="C15" t="str">
         <f>IF(En!B15&lt;&gt;0,En!B15,"")</f>
@@ -9582,7 +9588,7 @@
         <v>pref_app_show_sent_sms</v>
       </c>
       <c r="B16" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="C16" t="str">
         <f>IF(En!B16&lt;&gt;0,En!B16,"")</f>
@@ -9595,7 +9601,7 @@
         <v>pref_app_show_sent_sms_help</v>
       </c>
       <c r="B17" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="C17" t="str">
         <f>IF(En!B17&lt;&gt;0,En!B17,"")</f>
@@ -9608,7 +9614,7 @@
         <v>pref_app_call_logs_number</v>
       </c>
       <c r="B18" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="C18" t="str">
         <f>IF(En!B18&lt;&gt;0,En!B18,"")</f>
@@ -9621,7 +9627,7 @@
         <v>pref_app_call_logs_number_help</v>
       </c>
       <c r="B19" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="C19" t="str">
         <f>IF(En!B19&lt;&gt;0,En!B19,"")</f>
@@ -9634,7 +9640,7 @@
         <v>pref_app_ringtone</v>
       </c>
       <c r="B20" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="C20" t="str">
         <f>IF(En!B20&lt;&gt;0,En!B20,"")</f>
@@ -9647,7 +9653,7 @@
         <v>pref_app_ringtone_help</v>
       </c>
       <c r="B21" t="s">
-        <v>461</v>
+        <v>582</v>
       </c>
       <c r="C21" t="str">
         <f>IF(En!B21&lt;&gt;0,En!B21,"")</f>
@@ -9660,7 +9666,7 @@
         <v>pref_con</v>
       </c>
       <c r="B22" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="C22" t="str">
         <f>IF(En!B22&lt;&gt;0,En!B22,"")</f>
@@ -9673,7 +9679,7 @@
         <v>pref_con_notified_address_cat</v>
       </c>
       <c r="B23" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="C23" t="str">
         <f>IF(En!B23&lt;&gt;0,En!B23,"")</f>
@@ -9686,7 +9692,7 @@
         <v>pref_con_notified_address</v>
       </c>
       <c r="B24" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="C24" t="str">
         <f>IF(En!B24&lt;&gt;0,En!B24,"")</f>
@@ -9699,7 +9705,7 @@
         <v>pref_con_notified_address_help</v>
       </c>
       <c r="B25" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="C25" t="str">
         <f>IF(En!B25&lt;&gt;0,En!B25,"")</f>
@@ -9712,7 +9718,7 @@
         <v>pref_con_cat</v>
       </c>
       <c r="B26" t="s">
-        <v>462</v>
+        <v>583</v>
       </c>
       <c r="C26" t="str">
         <f>IF(En!B26&lt;&gt;0,En!B26,"")</f>
@@ -9725,7 +9731,7 @@
         <v>pref_con_use_different_account</v>
       </c>
       <c r="B27" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="C27" t="str">
         <f>IF(En!B27&lt;&gt;0,En!B27,"")</f>
@@ -9738,7 +9744,7 @@
         <v>pref_con_use_different_account_help</v>
       </c>
       <c r="B28" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="C28" t="str">
         <f>IF(En!B28&lt;&gt;0,En!B28,"")</f>
@@ -9764,7 +9770,7 @@
         <v>pref_con_login_help</v>
       </c>
       <c r="B30" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="C30" t="str">
         <f>IF(En!B30&lt;&gt;0,En!B30,"")</f>
@@ -9777,7 +9783,7 @@
         <v>pref_con_password</v>
       </c>
       <c r="B31" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="C31" t="str">
         <f>IF(En!B31&lt;&gt;0,En!B31,"")</f>
@@ -9790,7 +9796,7 @@
         <v>pref_con_password_help</v>
       </c>
       <c r="B32" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="C32" t="str">
         <f>IF(En!B32&lt;&gt;0,En!B32,"")</f>
@@ -9803,7 +9809,7 @@
         <v>pref_con_server_settings</v>
       </c>
       <c r="B33" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="C33" t="str">
         <f>IF(En!B33&lt;&gt;0,En!B33,"")</f>
@@ -9816,7 +9822,7 @@
         <v>pref_con_server_host</v>
       </c>
       <c r="B34" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="C34" t="str">
         <f>IF(En!B34&lt;&gt;0,En!B34,"")</f>
@@ -9829,7 +9835,7 @@
         <v>pref_con_server_host_help</v>
       </c>
       <c r="B35" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="C35" t="str">
         <f>IF(En!B35&lt;&gt;0,En!B35,"")</f>
@@ -9842,7 +9848,7 @@
         <v>pref_con_server_port</v>
       </c>
       <c r="B36" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="C36" t="str">
         <f>IF(En!B36&lt;&gt;0,En!B36,"")</f>
@@ -9855,7 +9861,7 @@
         <v>pref_con_server_port_help</v>
       </c>
       <c r="B37" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="C37" t="str">
         <f>IF(En!B37&lt;&gt;0,En!B37,"")</f>
@@ -9868,7 +9874,7 @@
         <v>pref_con_service_name</v>
       </c>
       <c r="B38" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
       <c r="C38" t="str">
         <f>IF(En!B38&lt;&gt;0,En!B38,"")</f>
@@ -9881,7 +9887,7 @@
         <v>pref_con_service_name_help</v>
       </c>
       <c r="B39" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="C39" t="str">
         <f>IF(En!B39&lt;&gt;0,En!B39,"")</f>
@@ -9894,7 +9900,7 @@
         <v>pref_notif</v>
       </c>
       <c r="B40" t="s">
-        <v>477</v>
+        <v>584</v>
       </c>
       <c r="C40" t="str">
         <f>IF(En!B40&lt;&gt;0,En!B40,"")</f>
@@ -9907,7 +9913,7 @@
         <v>pref_notif_application_connection</v>
       </c>
       <c r="B41" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="C41" t="str">
         <f>IF(En!B41&lt;&gt;0,En!B41,"")</f>
@@ -9920,7 +9926,7 @@
         <v>pref_notif_application_connection_help</v>
       </c>
       <c r="B42" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="C42" t="str">
         <f>IF(En!B42&lt;&gt;0,En!B42,"")</f>
@@ -9933,7 +9939,7 @@
         <v>pref_notif_battery_state</v>
       </c>
       <c r="B43" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="C43" t="str">
         <f>IF(En!B43&lt;&gt;0,En!B43,"")</f>
@@ -9946,7 +9952,7 @@
         <v>pref_notif_battery_state_help</v>
       </c>
       <c r="B44" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="C44" t="str">
         <f>IF(En!B44&lt;&gt;0,En!B44,"")</f>
@@ -9959,7 +9965,7 @@
         <v>pref_notif_battery_notif_interval</v>
       </c>
       <c r="B45" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="C45" t="str">
         <f>IF(En!B45&lt;&gt;0,En!B45,"")</f>
@@ -9972,7 +9978,7 @@
         <v>pref_notif_battery_notif_interval_help</v>
       </c>
       <c r="B46" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="C46" t="str">
         <f>IF(En!B46&lt;&gt;0,En!B46,"")</f>
@@ -9985,7 +9991,7 @@
         <v>pref_notif_battery_state_in_status</v>
       </c>
       <c r="B47" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="C47" t="str">
         <f>IF(En!B47&lt;&gt;0,En!B47,"")</f>
@@ -9998,7 +10004,7 @@
         <v>pref_notif_battery_state_in_status_help</v>
       </c>
       <c r="B48" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="C48" t="str">
         <f>IF(En!B48&lt;&gt;0,En!B48,"")</f>
@@ -10011,7 +10017,7 @@
         <v>pref_notif_incoming_sms</v>
       </c>
       <c r="B49" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="C49" t="str">
         <f>IF(En!B49&lt;&gt;0,En!B49,"")</f>
@@ -10024,7 +10030,7 @@
         <v>pref_notif_incoming_sms_help</v>
       </c>
       <c r="B50" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="C50" t="str">
         <f>IF(En!B50&lt;&gt;0,En!B50,"")</f>
@@ -10037,7 +10043,7 @@
         <v>pref_notif_incoming_calls</v>
       </c>
       <c r="B51" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="C51" t="str">
         <f>IF(En!B51&lt;&gt;0,En!B51,"")</f>
@@ -10050,7 +10056,7 @@
         <v>pref_notif_incoming_calls_help</v>
       </c>
       <c r="B52" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="C52" t="str">
         <f>IF(En!B52&lt;&gt;0,En!B52,"")</f>
@@ -10063,7 +10069,7 @@
         <v>pref_notif_sms_sent</v>
       </c>
       <c r="B53" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="C53" t="str">
         <f>IF(En!B53&lt;&gt;0,En!B53,"")</f>
@@ -10076,7 +10082,7 @@
         <v>pref_notif_sms_sent_help</v>
       </c>
       <c r="B54" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="C54" t="str">
         <f>IF(En!B54&lt;&gt;0,En!B54,"")</f>
@@ -10089,7 +10095,7 @@
         <v>pref_notif_sms_delivered</v>
       </c>
       <c r="B55" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="C55" t="str">
         <f>IF(En!B55&lt;&gt;0,En!B55,"")</f>
@@ -10102,7 +10108,7 @@
         <v>pref_notif_sms_delivered_help</v>
       </c>
       <c r="B56" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="C56" t="str">
         <f>IF(En!B56&lt;&gt;0,En!B56,"")</f>
@@ -10128,7 +10134,7 @@
         <v>main_but_preferences</v>
       </c>
       <c r="B58" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="C58" t="str">
         <f>IF(En!B58&lt;&gt;0,En!B58,"")</f>
@@ -10141,7 +10147,7 @@
         <v>main_but_send_clipboard</v>
       </c>
       <c r="B59" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="C59" t="str">
         <f>IF(En!B59&lt;&gt;0,En!B59,"")</f>
@@ -10154,7 +10160,7 @@
         <v>main_but_about</v>
       </c>
       <c r="B60" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="C60" t="str">
         <f>IF(En!B60&lt;&gt;0,En!B60,"")</f>
@@ -10180,7 +10186,7 @@
         <v>about_panel</v>
       </c>
       <c r="B62" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="C62" t="str">
         <f>IF(En!B62&lt;&gt;0,En!B62,"")</f>
@@ -10206,7 +10212,7 @@
         <v>preference_panel</v>
       </c>
       <c r="B64" t="s">
-        <v>441</v>
+        <v>585</v>
       </c>
       <c r="C64" t="str">
         <f>IF(En!B64&lt;&gt;0,En!B64,"")</f>
@@ -10219,7 +10225,7 @@
         <v>log_panel_acquiring</v>
       </c>
       <c r="B65" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="C65" t="str">
         <f>IF(En!B65&lt;&gt;0,En!B65,"")</f>
@@ -10232,7 +10238,7 @@
         <v>log_panel_collect</v>
       </c>
       <c r="B66" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
       <c r="C66" t="str">
         <f>IF(En!B66&lt;&gt;0,En!B66,"")</f>
@@ -10245,7 +10251,7 @@
         <v>main_service_connected</v>
       </c>
       <c r="B67" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="C67" t="str">
         <f>IF(En!B67&lt;&gt;0,En!B67,"")</f>
@@ -10258,7 +10264,7 @@
         <v>main_service_connecting</v>
       </c>
       <c r="B68" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="C68" t="str">
         <f>IF(En!B68&lt;&gt;0,En!B68,"")</f>
@@ -10271,7 +10277,7 @@
         <v>main_service_disconnected</v>
       </c>
       <c r="B69" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="C69" t="str">
         <f>IF(En!B69&lt;&gt;0,En!B69,"")</f>
@@ -10284,7 +10290,7 @@
         <v>main_service_disconnecting</v>
       </c>
       <c r="B70" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="C70" t="str">
         <f>IF(En!B70&lt;&gt;0,En!B70,"")</f>
@@ -10297,7 +10303,7 @@
         <v>main_service_waiting</v>
       </c>
       <c r="B71" t="s">
-        <v>503</v>
+        <v>586</v>
       </c>
       <c r="C71" t="str">
         <f>IF(En!B71&lt;&gt;0,En!B71,"")</f>
@@ -10310,7 +10316,7 @@
         <v>main_service_waiting_to_connect</v>
       </c>
       <c r="B72" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="C72" t="str">
         <f>IF(En!B72&lt;&gt;0,En!B72,"")</f>
@@ -10323,7 +10329,7 @@
         <v>main_service_stop</v>
       </c>
       <c r="B73" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="C73" t="str">
         <f>IF(En!B73&lt;&gt;0,En!B73,"")</f>
@@ -10336,7 +10342,7 @@
         <v>xmpp_manager_reconnecting</v>
       </c>
       <c r="B74" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="C74" t="str">
         <f>IF(En!B74&lt;&gt;0,En!B74,"")</f>
@@ -10349,7 +10355,7 @@
         <v>xmpp_manager_failed_max_attempts</v>
       </c>
       <c r="B75" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="C75" t="str">
         <f>IF(En!B75&lt;&gt;0,En!B75,"")</f>
@@ -10362,7 +10368,7 @@
         <v>xmpp_manager_waiting</v>
       </c>
       <c r="B76" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="C76" t="str">
         <f>IF(En!B76&lt;&gt;0,En!B76,"")</f>
@@ -10375,7 +10381,7 @@
         <v>xmpp_manager_connection_failed</v>
       </c>
       <c r="B77" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="C77" t="str">
         <f>IF(En!B77&lt;&gt;0,En!B77,"")</f>
@@ -10388,7 +10394,7 @@
         <v>xmpp_manager_login_failed</v>
       </c>
       <c r="B78" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="C78" t="str">
         <f>IF(En!B78&lt;&gt;0,En!B78,"")</f>
@@ -10401,7 +10407,7 @@
         <v>xmpp_manager_invalid_credentials</v>
       </c>
       <c r="B79" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="C79" t="str">
         <f>IF(En!B79&lt;&gt;0,En!B79,"")</f>
@@ -10427,7 +10433,7 @@
         <v>about_authors</v>
       </c>
       <c r="B81" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="C81" t="str">
         <f>IF(En!B81&lt;&gt;0,En!B81,"")</f>
@@ -10440,7 +10446,7 @@
         <v>about_donors</v>
       </c>
       <c r="B82" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C82" t="str">
         <f>IF(En!B82&lt;&gt;0,En!B82,"")</f>
@@ -10453,7 +10459,7 @@
         <v>about_change_log</v>
       </c>
       <c r="B83" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C83" t="str">
         <f>IF(En!B83&lt;&gt;0,En!B83,"")</f>
@@ -10466,7 +10472,7 @@
         <v>chat_sms_from</v>
       </c>
       <c r="B84" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C84" t="str">
         <f>IF(En!B84&lt;&gt;0,En!B84,"")</f>
@@ -10479,7 +10485,7 @@
         <v>chat_battery_level</v>
       </c>
       <c r="B85" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="C85" t="str">
         <f>IF(En!B85&lt;&gt;0,En!B85,"")</f>
@@ -10492,7 +10498,7 @@
         <v>chat_error_no_recipient</v>
       </c>
       <c r="B86" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="C86" t="str">
         <f>IF(En!B86&lt;&gt;0,En!B86,"")</f>
@@ -10505,7 +10511,7 @@
         <v>chat_error_unknown_cmd</v>
       </c>
       <c r="B87" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="C87" t="str">
         <f>IF(En!B87&lt;&gt;0,En!B87,"")</f>
@@ -10518,7 +10524,7 @@
         <v>chat_error</v>
       </c>
       <c r="B88" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
       <c r="C88" t="str">
         <f>IF(En!B88&lt;&gt;0,En!B88,"")</f>
@@ -10531,7 +10537,7 @@
         <v>chat_error_root</v>
       </c>
       <c r="B89" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="C89" t="str">
         <f>IF(En!B89&lt;&gt;0,En!B89,"")</f>
@@ -10544,7 +10550,7 @@
         <v>chat_reply_contact</v>
       </c>
       <c r="B90" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="C90" t="str">
         <f>IF(En!B90&lt;&gt;0,En!B90,"")</f>
@@ -10557,7 +10563,7 @@
         <v>chat_start_locating</v>
       </c>
       <c r="B91" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="C91" t="str">
         <f>IF(En!B91&lt;&gt;0,En!B91,"")</f>
@@ -10570,7 +10576,7 @@
         <v>chat_start_ringing</v>
       </c>
       <c r="B92" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="C92" t="str">
         <f>IF(En!B92&lt;&gt;0,En!B92,"")</f>
@@ -10583,7 +10589,7 @@
         <v>chat_error_ringing</v>
       </c>
       <c r="B93" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="C93" t="str">
         <f>IF(En!B93&lt;&gt;0,En!B93,"")</f>
@@ -10596,7 +10602,7 @@
         <v>chat_stop_actions</v>
       </c>
       <c r="B94" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="C94" t="str">
         <f>IF(En!B94&lt;&gt;0,En!B94,"")</f>
@@ -10609,11 +10615,11 @@
         <v>chat_send_sms</v>
       </c>
       <c r="B95" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="C95" t="str">
         <f>IF(En!B95&lt;&gt;0,En!B95,"")</f>
-        <v>Sending sms to %s</v>
+        <v>Sending SMS to %s</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -10622,7 +10628,7 @@
         <v>chat_specify_details</v>
       </c>
       <c r="B96" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="C96" t="str">
         <f>IF(En!B96&lt;&gt;0,En!B96,"")</f>
@@ -10635,7 +10641,7 @@
         <v>chat_no_match_for</v>
       </c>
       <c r="B97" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="C97" t="str">
         <f>IF(En!B97&lt;&gt;0,En!B97,"")</f>
@@ -10648,11 +10654,11 @@
         <v>chat_mark_as_read</v>
       </c>
       <c r="B98" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="C98" t="str">
         <f>IF(En!B98&lt;&gt;0,En!B98,"")</f>
-        <v>Mark %s\'s sms as read</v>
+        <v>Mark %s\'s SMS as read</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -10661,11 +10667,11 @@
         <v>chat_only_got_n_sms</v>
       </c>
       <c r="B99" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="C99" t="str">
         <f>IF(En!B99&lt;&gt;0,En!B99,"")</f>
-        <v>Only got %d sms</v>
+        <v>Only got %d SMS</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -10674,11 +10680,11 @@
         <v>chat_no_sms</v>
       </c>
       <c r="B100" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="C100" t="str">
         <f>IF(En!B100&lt;&gt;0,En!B100,"")</f>
-        <v>No sms found</v>
+        <v>No SMS found</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -10687,7 +10693,7 @@
         <v>chat_no_call</v>
       </c>
       <c r="B101" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="C101" t="str">
         <f>IF(En!B101&lt;&gt;0,En!B101,"")</f>
@@ -10700,7 +10706,7 @@
         <v>chat_contact_found</v>
       </c>
       <c r="B102" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="C102" t="str">
         <f>IF(En!B102&lt;&gt;0,En!B102,"")</f>
@@ -10713,7 +10719,7 @@
         <v>chat_phones</v>
       </c>
       <c r="B103" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="C103" t="str">
         <f>IF(En!B103&lt;&gt;0,En!B103,"")</f>
@@ -10726,7 +10732,7 @@
         <v>chat_emails</v>
       </c>
       <c r="B104" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="C104" t="str">
         <f>IF(En!B104&lt;&gt;0,En!B104,"")</f>
@@ -10739,7 +10745,7 @@
         <v>chat_addresses</v>
       </c>
       <c r="B105" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="C105" t="str">
         <f>IF(En!B105&lt;&gt;0,En!B105,"")</f>
@@ -10752,7 +10758,7 @@
         <v>chat_text_copied</v>
       </c>
       <c r="B106" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="C106" t="str">
         <f>IF(En!B106&lt;&gt;0,En!B106,"")</f>
@@ -10765,7 +10771,7 @@
         <v>chat_error_clipboard</v>
       </c>
       <c r="B107" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="C107" t="str">
         <f>IF(En!B107&lt;&gt;0,En!B107,"")</f>
@@ -10778,7 +10784,7 @@
         <v>chat_clipboard</v>
       </c>
       <c r="B108" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="C108" t="str">
         <f>IF(En!B108&lt;&gt;0,En!B108,"")</f>
@@ -10791,7 +10797,7 @@
         <v>chat_choose_activity</v>
       </c>
       <c r="B109" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="C109" t="str">
         <f>IF(En!B109&lt;&gt;0,En!B109,"")</f>
@@ -10804,7 +10810,7 @@
         <v>chat_dial</v>
       </c>
       <c r="B110" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="C110" t="str">
         <f>IF(En!B110&lt;&gt;0,En!B110,"")</f>
@@ -10817,7 +10823,7 @@
         <v>chat_error_dial</v>
       </c>
       <c r="B111" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="C111" t="str">
         <f>IF(En!B111&lt;&gt;0,En!B111,"")</f>
@@ -10830,7 +10836,7 @@
         <v>chat_help_title</v>
       </c>
       <c r="B112" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="C112" t="str">
         <f>IF(En!B112&lt;&gt;0,En!B112,"")</f>
@@ -10843,7 +10849,7 @@
         <v>chat_help_help</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="C113" t="str">
         <f>IF(En!B113&lt;&gt;0,En!B113,"")</f>
@@ -10856,7 +10862,7 @@
         <v>chat_help_stop</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="C114" t="str">
         <f>IF(En!B114&lt;&gt;0,En!B114,"")</f>
@@ -10869,7 +10875,7 @@
         <v>chat_help_dial</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="C115" t="str">
         <f>IF(En!B115&lt;&gt;0,En!B115,"")</f>
@@ -10882,11 +10888,11 @@
         <v>chat_help_sms_reply</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="C116" t="str">
         <f>IF(En!B116&lt;&gt;0,En!B116,"")</f>
-        <v>- %s: send a sms to your last recipient with content message.</v>
+        <v>- %s: send a SMS to your last recipient with content message.</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -10895,11 +10901,11 @@
         <v>chat_help_sms_show_all</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="C117" t="str">
         <f>IF(En!B117&lt;&gt;0,En!B117,"")</f>
-        <v>- %s: display last sent sms from all contact.</v>
+        <v>- %s: display last sent SMS from all contact.</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -10908,11 +10914,11 @@
         <v>chat_help_sms_show_contact</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="C118" t="str">
         <f>IF(En!B118&lt;&gt;0,En!B118,"")</f>
-        <v>- %s: display last sent sms from searched contacts.</v>
+        <v>- %s: display last sent SMS from searched contacts.</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -10921,11 +10927,11 @@
         <v>chat_help_sms_send</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="C119" t="str">
         <f>IF(En!B119&lt;&gt;0,En!B119,"")</f>
-        <v>- %s: sends a sms to number with content message.</v>
+        <v>- %s: sends a SMS to number with content message.</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -10934,11 +10940,11 @@
         <v>chat_help_mark_as_read</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="C120" t="str">
         <f>IF(En!B120&lt;&gt;0,En!B120,"")</f>
-        <v>- %1$s or %2$s: mark sms as read for last recipient or given contact.</v>
+        <v>- %1$s or %2$s: mark SMS as read for last recipient or given contact.</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -10947,7 +10953,7 @@
         <v>chat_help_battery</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="C121" t="str">
         <f>IF(En!B121&lt;&gt;0,En!B121,"")</f>
@@ -10960,7 +10966,7 @@
         <v>chat_help_calls</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C122" t="str">
         <f>IF(En!B122&lt;&gt;0,En!B122,"")</f>
@@ -10973,7 +10979,7 @@
         <v>chat_help_contact</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="C123" t="str">
         <f>IF(En!B123&lt;&gt;0,En!B123,"")</f>
@@ -10986,7 +10992,7 @@
         <v>chat_help_geo</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="C124" t="str">
         <f>IF(En!B124&lt;&gt;0,En!B124,"")</f>
@@ -10999,7 +11005,7 @@
         <v>chat_help_where</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="C125" t="str">
         <f>IF(En!B125&lt;&gt;0,En!B125,"")</f>
@@ -11012,7 +11018,7 @@
         <v>chat_help_ring</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="C126" t="str">
         <f>IF(En!B126&lt;&gt;0,En!B126,"")</f>
@@ -11025,7 +11031,7 @@
         <v>chat_help_copy</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="C127" t="str">
         <f>IF(En!B127&lt;&gt;0,En!B127,"")</f>
@@ -11038,7 +11044,7 @@
         <v>chat_help_cmd</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="C128" t="str">
         <f>IF(En!B128&lt;&gt;0,En!B128,"")</f>
@@ -11051,7 +11057,7 @@
         <v>chat_help_write</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="C129" t="str">
         <f>IF(En!B129&lt;&gt;0,En!B129,"")</f>
@@ -11064,7 +11070,7 @@
         <v>chat_help_urls</v>
       </c>
       <c r="B130" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="C130" t="str">
         <f>IF(En!B130&lt;&gt;0,En!B130,"")</f>
@@ -11077,7 +11083,7 @@
         <v>chat_call_unknown</v>
       </c>
       <c r="B131" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="C131" t="str">
         <f>IF(En!B131&lt;&gt;0,En!B131,"")</f>
@@ -11090,7 +11096,7 @@
         <v>chat_call_incoming</v>
       </c>
       <c r="B132" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="C132" t="str">
         <f>IF(En!B132&lt;&gt;0,En!B132,"")</f>
@@ -11103,7 +11109,7 @@
         <v>chat_call_outgoing</v>
       </c>
       <c r="B133" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="C133" t="str">
         <f>IF(En!B133&lt;&gt;0,En!B133,"")</f>
@@ -11116,7 +11122,7 @@
         <v>chat_call_missed</v>
       </c>
       <c r="B134" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="C134" t="str">
         <f>IF(En!B134&lt;&gt;0,En!B134,"")</f>
@@ -11129,7 +11135,7 @@
         <v>chat_call_duration</v>
       </c>
       <c r="B135" t="s">
-        <v>566</v>
+        <v>553</v>
       </c>
       <c r="C135" t="str">
         <f>IF(En!B135&lt;&gt;0,En!B135,"")</f>
@@ -11142,7 +11148,7 @@
         <v>chat_welcome</v>
       </c>
       <c r="B136" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C136" t="str">
         <f>IF(En!B136&lt;&gt;0,En!B136,"")</f>
@@ -11155,7 +11161,7 @@
         <v>chat_app_stop</v>
       </c>
       <c r="B137" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="C137" t="str">
         <f>IF(En!B137&lt;&gt;0,En!B137,"")</f>
@@ -11168,7 +11174,7 @@
         <v>chat_is_calling</v>
       </c>
       <c r="B138" t="s">
-        <v>569</v>
+        <v>556</v>
       </c>
       <c r="C138" t="str">
         <f>IF(En!B138&lt;&gt;0,En!B138,"")</f>
@@ -11181,7 +11187,7 @@
         <v>chat_call_hidden</v>
       </c>
       <c r="B139" t="s">
-        <v>570</v>
+        <v>557</v>
       </c>
       <c r="C139" t="str">
         <f>IF(En!B139&lt;&gt;0,En!B139,"")</f>
@@ -11194,7 +11200,7 @@
         <v>chat_sms_sent</v>
       </c>
       <c r="B140" t="s">
-        <v>571</v>
+        <v>558</v>
       </c>
       <c r="C140" t="str">
         <f>IF(En!B140&lt;&gt;0,En!B140,"")</f>
@@ -11207,7 +11213,7 @@
         <v>chat_sms_failure</v>
       </c>
       <c r="B141" t="s">
-        <v>572</v>
+        <v>559</v>
       </c>
       <c r="C141" t="str">
         <f>IF(En!B141&lt;&gt;0,En!B141,"")</f>
@@ -11220,7 +11226,7 @@
         <v>chat_sms_no_service</v>
       </c>
       <c r="B142" t="s">
-        <v>573</v>
+        <v>560</v>
       </c>
       <c r="C142" t="str">
         <f>IF(En!B142&lt;&gt;0,En!B142,"")</f>
@@ -11233,7 +11239,7 @@
         <v>chat_sms_null_pdu</v>
       </c>
       <c r="B143" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="C143" t="str">
         <f>IF(En!B143&lt;&gt;0,En!B143,"")</f>
@@ -11246,7 +11252,7 @@
         <v>chat_sms_radio_off</v>
       </c>
       <c r="B144" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="C144" t="str">
         <f>IF(En!B144&lt;&gt;0,En!B144,"")</f>
@@ -11259,7 +11265,7 @@
         <v>chat_sms_delivered</v>
       </c>
       <c r="B145" t="s">
-        <v>576</v>
+        <v>563</v>
       </c>
       <c r="C145" t="str">
         <f>IF(En!B145&lt;&gt;0,En!B145,"")</f>
@@ -11272,7 +11278,7 @@
         <v>chat_sms_not_delivered</v>
       </c>
       <c r="B146" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="C146" t="str">
         <f>IF(En!B146&lt;&gt;0,En!B146,"")</f>
@@ -11285,7 +11291,7 @@
         <v>chat_log_failed</v>
       </c>
       <c r="B147" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
       <c r="C147" t="str">
         <f>IF(En!B147&lt;&gt;0,En!B147,"")</f>
@@ -11298,7 +11304,7 @@
         <v>chat_log_unavailable</v>
       </c>
       <c r="B148" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="C148" t="str">
         <f>IF(En!B148&lt;&gt;0,En!B148,"")</f>
@@ -11311,7 +11317,7 @@
         <v>chat_geo_accuracy</v>
       </c>
       <c r="B149" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="C149" t="str">
         <f>IF(En!B149&lt;&gt;0,En!B149,"")</f>
@@ -11324,7 +11330,7 @@
         <v>chat_geo_altitude</v>
       </c>
       <c r="B150" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="C150" t="str">
         <f>IF(En!B150&lt;&gt;0,En!B150,"")</f>
@@ -11337,7 +11343,7 @@
         <v>chat_geo_speed</v>
       </c>
       <c r="B151" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="C151" t="str">
         <f>IF(En!B151&lt;&gt;0,En!B151,"")</f>
@@ -11350,7 +11356,7 @@
         <v>chat_geo_provider</v>
       </c>
       <c r="B152" t="s">
-        <v>583</v>
+        <v>570</v>
       </c>
       <c r="C152" t="str">
         <f>IF(En!B152&lt;&gt;0,En!B152,"")</f>
@@ -11363,7 +11369,7 @@
         <v>pref_app_locale</v>
       </c>
       <c r="B153" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="C153" t="str">
         <f>IF(En!B153&lt;&gt;0,En!B153,"")</f>
@@ -11376,7 +11382,7 @@
         <v>pref_app_locale_help</v>
       </c>
       <c r="B154" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="C154" t="str">
         <f>IF(En!B154&lt;&gt;0,En!B154,"")</f>
@@ -15345,6 +15351,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17448,7 +17455,7 @@
       </c>
       <c r="D95" t="str">
         <f>IF(En!B95&lt;&gt;0,En!B95,"")</f>
-        <v>Sending sms to %s</v>
+        <v>Sending SMS to %s</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="5"/>
@@ -17514,7 +17521,7 @@
       </c>
       <c r="D98" t="str">
         <f>IF(En!B98&lt;&gt;0,En!B98,"")</f>
-        <v>Mark %s\'s sms as read</v>
+        <v>Mark %s\'s SMS as read</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="5"/>
@@ -17536,7 +17543,7 @@
       </c>
       <c r="D99" t="str">
         <f>IF(En!B99&lt;&gt;0,En!B99,"")</f>
-        <v>Only got %d sms</v>
+        <v>Only got %d SMS</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="5"/>
@@ -17558,7 +17565,7 @@
       </c>
       <c r="D100" t="str">
         <f>IF(En!B100&lt;&gt;0,En!B100,"")</f>
-        <v>No sms found</v>
+        <v>No SMS found</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="5"/>
@@ -17910,7 +17917,7 @@
       </c>
       <c r="D116" t="str">
         <f>IF(En!B116&lt;&gt;0,En!B116,"")</f>
-        <v>- %s: send a sms to your last recipient with content message.</v>
+        <v>- %s: send a SMS to your last recipient with content message.</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="5"/>
@@ -17932,7 +17939,7 @@
       </c>
       <c r="D117" t="str">
         <f>IF(En!B117&lt;&gt;0,En!B117,"")</f>
-        <v>- %s: display last sent sms from all contact.</v>
+        <v>- %s: display last sent SMS from all contact.</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="5"/>
@@ -17954,7 +17961,7 @@
       </c>
       <c r="D118" t="str">
         <f>IF(En!B118&lt;&gt;0,En!B118,"")</f>
-        <v>- %s: display last sent sms from searched contacts.</v>
+        <v>- %s: display last sent SMS from searched contacts.</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="5"/>
@@ -17976,7 +17983,7 @@
       </c>
       <c r="D119" t="str">
         <f>IF(En!B119&lt;&gt;0,En!B119,"")</f>
-        <v>- %s: sends a sms to number with content message.</v>
+        <v>- %s: sends a SMS to number with content message.</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="5"/>
@@ -17998,7 +18005,7 @@
       </c>
       <c r="D120" t="str">
         <f>IF(En!B120&lt;&gt;0,En!B120,"")</f>
-        <v>- %1$s or %2$s: mark sms as read for last recipient or given contact.</v>
+        <v>- %1$s or %2$s: mark SMS as read for last recipient or given contact.</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="5"/>
@@ -36824,8 +36831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E480"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E154" sqref="A1:E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -37160,7 +37167,7 @@
       </c>
       <c r="D15" t="str">
         <f>IF(De!B15&lt;&gt;0,De!B15,"")</f>
-        <v xml:space="preserve">Anzahl der SMS gezeigt werden </v>
+        <v>Anzahl der SMS die ausgegeben werden</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="2"/>
@@ -37292,7 +37299,7 @@
       </c>
       <c r="D21" t="str">
         <f>IF(De!B21&lt;&gt;0,De!B21,"")</f>
-        <v>Klingelton der durch den ring Befehl abgespielt wird</v>
+        <v>Klingelton der durch den \"ring\" Befehl abgespielt wird</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="2"/>
@@ -37402,7 +37409,7 @@
       </c>
       <c r="D26" t="str">
         <f>IF(De!B26&lt;&gt;0,De!B26,"")</f>
-        <v>Verbindungseinstellungen</v>
+        <v>Verbindungsoptionen</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="2"/>
@@ -37710,7 +37717,7 @@
       </c>
       <c r="D40" t="str">
         <f>IF(De!B40&lt;&gt;0,De!B40,"")</f>
-        <v>Benachrichtigungseinstellungen</v>
+        <v>Benachrichtigungsoptionen</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="2"/>
@@ -38238,7 +38245,7 @@
       </c>
       <c r="D64" t="str">
         <f>IF(De!B64&lt;&gt;0,De!B64,"")</f>
-        <v>Einstellungen</v>
+        <v>Anwendungsoptionen</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="2"/>
@@ -38392,7 +38399,7 @@
       </c>
       <c r="D71" t="str">
         <f>IF(De!B71&lt;&gt;0,De!B71,"")</f>
-        <v>Warte...</v>
+        <v>Wartend...</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="5"/>

</xml_diff>